<commit_message>
wip: read text in file
</commit_message>
<xml_diff>
--- a/temp_results.xlsx
+++ b/temp_results.xlsx
@@ -619,7 +619,11 @@
       </c>
       <c r="S2" t="inlineStr"/>
       <c r="T2" t="inlineStr"/>
-      <c r="U2" t="inlineStr"/>
+      <c r="U2" t="inlineStr">
+        <is>
+          <t>Others</t>
+        </is>
+      </c>
       <c r="V2" t="inlineStr"/>
       <c r="W2" t="inlineStr">
         <is>

</xml_diff>